<commit_message>
GNUPlot e Gráficos ISCC
</commit_message>
<xml_diff>
--- a/intervalos_ndt_10.98.xlsx
+++ b/intervalos_ndt_10.98.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wsl_atual\simulador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE9ABF1-E2D6-45B4-8619-B748CDFC55B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47E5FE6-E562-4972-B026-9E84639F7C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F3419C55-1066-4486-8782-759DF9273BDF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{F3419C55-1066-4486-8782-759DF9273BDF}"/>
   </bookViews>
   <sheets>
     <sheet name="10.98 x 10.98" sheetId="4" r:id="rId1"/>
@@ -8239,16 +8239,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95251</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>83343</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>11905</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8280,16 +8280,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>119061</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>261937</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8321,16 +8321,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>254793</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>264318</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8362,16 +8362,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>397669</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>83343</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>297656</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8698,7 +8698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7747BC58-7A05-4AFD-AFFF-668AA696D33C}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -9089,7 +9089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1A77DB-ED1E-4FD8-912B-B7724CE6C6D1}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:B68"/>
     </sheetView>
   </sheetViews>
@@ -9645,7 +9645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45111533-F0D8-4E2A-AC2C-0F519570E293}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
@@ -10082,7 +10082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA0AEAA-9F06-41FA-95F7-2C4DA2E0B603}">
   <dimension ref="A1:B941"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>

</xml_diff>